<commit_message>
test with complex formula
</commit_message>
<xml_diff>
--- a/assessments/tests/resources/score_sheet_with_formula.xlsx
+++ b/assessments/tests/resources/score_sheet_with_formula.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="majeurs+mineurs" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <t xml:space="preserve">2017-18 – LOSIS1211</t>
   </si>
@@ -107,6 +108,21 @@
   </si>
   <si>
     <t xml:space="preserve">John</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Etude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Résultat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note finale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smith, Adam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doe, John</t>
   </si>
 </sst>
 </file>
@@ -490,7 +506,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -606,7 +622,7 @@
         <v>24</v>
       </c>
       <c r="H12" s="0" t="n">
-        <f aca="false">MAX(1,5,10,15)</f>
+        <f aca="false">VLOOKUP(E12,'majeurs+mineurs'!$A$2:$E$3,5,0)</f>
         <v>15</v>
       </c>
       <c r="J12" s="2" t="s">
@@ -639,6 +655,7 @@
         <v>28</v>
       </c>
       <c r="H13" s="0" t="n">
+        <f aca="false">MAX(1,12,17)</f>
         <v>17</v>
       </c>
       <c r="J13" s="2" t="s">
@@ -672,4 +689,84 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="9.14"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>14.7</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <f aca="false">ROUND(D2,0)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>17.1</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <f aca="false">ROUND(D3,0)</f>
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>